<commit_message>
Fix way point selection bugs
</commit_message>
<xml_diff>
--- a/towns3.0.xlsx
+++ b/towns3.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zissou/Downloads/RouteFinder-master/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zissou/Library/Mobile Documents/com~apple~CloudDocs/College/YearTwo/SemesterTwo/DSII/code/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113AAE15-AAAA-324C-8BCB-0DBB39BE6B36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7740442-7BAE-3847-9C8C-F4A8213E6B37}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" activeTab="1" xr2:uid="{DBCE131A-A3CE-4E2D-AF18-B48AB3E1F46A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{DBCE131A-A3CE-4E2D-AF18-B48AB3E1F46A}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
@@ -577,8 +577,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T146"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D20" sqref="D1:D1048576"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1461,10 +1461,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DA4984-602A-D449-B363-ADE69DAEFD28}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D160"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="F95" sqref="F95"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3709,6 +3709,20 @@
         <v>21</v>
       </c>
     </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>60</v>
+      </c>
+      <c r="B161">
+        <v>57</v>
+      </c>
+      <c r="C161">
+        <v>14</v>
+      </c>
+      <c r="D161">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:D161">
     <sortCondition ref="B1"/>

</xml_diff>